<commit_message>
V1.1 Fantasy App - add Estadisticas and Torneos
</commit_message>
<xml_diff>
--- a/gronestats/data/master_data/BD Alkagrone 2025.xlsx
+++ b/gronestats/data/master_data/BD Alkagrone 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStatz\gronestats\data\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23FB680-9894-4146-9C2D-3A17FEB24E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C390922-1BC4-40D3-B331-63E05A42672D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="9" xr2:uid="{04309B13-EF36-4AA6-8981-9F5853643808}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" firstSheet="4" activeTab="9" xr2:uid="{04309B13-EF36-4AA6-8981-9F5853643808}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla_Acumulada" sheetId="15" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3479" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3493" uniqueCount="1119">
   <si>
     <t>ADT</t>
   </si>
@@ -3392,6 +3392,18 @@
   </si>
   <si>
     <t>Descalificado</t>
+  </si>
+  <si>
+    <t>Héroes de San Ramón</t>
+  </si>
+  <si>
+    <t>CD Moquegua</t>
+  </si>
+  <si>
+    <t>FC Cajamarca</t>
+  </si>
+  <si>
+    <t>Moquegua</t>
   </si>
 </sst>
 </file>
@@ -3682,7 +3694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3840,6 +3852,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -7287,8 +7302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9E1391-B1F8-4774-8842-076EACF1F12E}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8021,6 +8036,58 @@
       </c>
       <c r="K20" s="2" t="s">
         <v>450</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>492848</v>
+      </c>
+      <c r="B21" s="61" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>437</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>1082002</v>
+      </c>
+      <c r="B22" s="61" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>437</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -8684,10 +8751,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97128C34-A586-46D1-9E7A-99D80688965C}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9018,8 +9085,25 @@
         <v>18080</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>319</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C20" s="35">
+        <v>2750</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E20" s="35">
+        <v>11000</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E19">
+  <conditionalFormatting sqref="E2:E20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>